<commit_message>
Fix demographics tab; Add 2020 multi-year groupings
</commit_message>
<xml_diff>
--- a/myCCB/myInfo/County Codes to County Names Linkage.xlsx
+++ b/myCCB/myInfo/County Codes to County Names Linkage.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\0.CBD\myCBD\myInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\FusionData\0.CCB\myCCB\myInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D774BEFE-11C6-4B35-BA88-29214180764B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8175"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="222">
   <si>
     <t>countyName</t>
   </si>
@@ -657,12 +658,45 @@
   </si>
   <si>
     <t>GOLD COAST</t>
+  </si>
+  <si>
+    <t>REGION_CENSUS</t>
+  </si>
+  <si>
+    <t>San Francisco Bay Area</t>
+  </si>
+  <si>
+    <t>Superior CA</t>
+  </si>
+  <si>
+    <t>North Coast</t>
+  </si>
+  <si>
+    <t>Northern San Joaquin Valley</t>
+  </si>
+  <si>
+    <t>Central Coast</t>
+  </si>
+  <si>
+    <t>Southern San Joaquin Valley</t>
+  </si>
+  <si>
+    <t>Inland Empire</t>
+  </si>
+  <si>
+    <t>Los Angeles County</t>
+  </si>
+  <si>
+    <t>Orange County</t>
+  </si>
+  <si>
+    <t>San Diego - Imperial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -974,11 +1008,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J59"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="N51" sqref="N51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,9 +1027,10 @@
     <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="46.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1026,8 +1061,11 @@
       <c r="J1" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1058,8 +1096,11 @@
       <c r="J2" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1090,8 +1131,11 @@
       <c r="J3" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1122,8 +1166,11 @@
       <c r="J4" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1154,8 +1201,11 @@
       <c r="J5" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1186,8 +1236,11 @@
       <c r="J6" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1218,8 +1271,11 @@
       <c r="J7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1250,8 +1306,11 @@
       <c r="J8" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1282,8 +1341,11 @@
       <c r="J9" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1314,8 +1376,11 @@
       <c r="J10" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1346,8 +1411,11 @@
       <c r="J11" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1378,8 +1446,11 @@
       <c r="J12" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1410,8 +1481,11 @@
       <c r="J13" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1442,8 +1516,11 @@
       <c r="J14" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -1474,8 +1551,11 @@
       <c r="J15" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1506,8 +1586,11 @@
       <c r="J16" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -1538,8 +1621,11 @@
       <c r="J17" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1570,8 +1656,11 @@
       <c r="J18" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1602,8 +1691,11 @@
       <c r="J19" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -1634,8 +1726,11 @@
       <c r="J20" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1666,8 +1761,11 @@
       <c r="J21" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1698,8 +1796,11 @@
       <c r="J22" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1730,8 +1831,11 @@
       <c r="J23" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>82</v>
       </c>
@@ -1762,8 +1866,11 @@
       <c r="J24" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1794,8 +1901,11 @@
       <c r="J25" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1826,8 +1936,11 @@
       <c r="J26" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1858,8 +1971,11 @@
       <c r="J27" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1890,8 +2006,11 @@
       <c r="J28" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K28" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1922,8 +2041,11 @@
       <c r="J29" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1954,8 +2076,11 @@
       <c r="J30" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1986,8 +2111,11 @@
       <c r="J31" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K31" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2018,8 +2146,11 @@
       <c r="J32" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2050,8 +2181,11 @@
       <c r="J33" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2082,8 +2216,11 @@
       <c r="J34" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2114,8 +2251,11 @@
       <c r="J35" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K35" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2146,8 +2286,11 @@
       <c r="J36" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>95</v>
       </c>
@@ -2178,8 +2321,11 @@
       <c r="J37" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K37" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2210,8 +2356,11 @@
       <c r="J38" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K38" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2242,8 +2391,11 @@
       <c r="J39" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K39" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2274,8 +2426,11 @@
       <c r="J40" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2306,8 +2461,11 @@
       <c r="J41" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2338,8 +2496,11 @@
       <c r="J42" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K42" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2370,8 +2531,11 @@
       <c r="J43" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K43" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2402,8 +2566,11 @@
       <c r="J44" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K44" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2434,8 +2601,11 @@
       <c r="J45" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K45" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2466,8 +2636,11 @@
       <c r="J46" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K46" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2498,8 +2671,11 @@
       <c r="J47" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K47" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2530,8 +2706,11 @@
       <c r="J48" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K48" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2562,8 +2741,11 @@
       <c r="J49" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K49" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2594,8 +2776,11 @@
       <c r="J50" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K50" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2626,8 +2811,11 @@
       <c r="J51" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K51" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2658,8 +2846,11 @@
       <c r="J52" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K52" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2690,8 +2881,11 @@
       <c r="J53" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K53" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2722,8 +2916,11 @@
       <c r="J54" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K54" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2754,8 +2951,11 @@
       <c r="J55" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K55" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2786,8 +2986,11 @@
       <c r="J56" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K56" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2818,8 +3021,11 @@
       <c r="J57" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K57" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2850,8 +3056,11 @@
       <c r="J58" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K58" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2881,6 +3090,9 @@
       </c>
       <c r="J59" t="s">
         <v>192</v>
+      </c>
+      <c r="K59" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>